<commit_message>
Added code to convert sheet into object[][]
</commit_message>
<xml_diff>
--- a/test-data/OrangeData.xlsx
+++ b/test-data/OrangeData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labuser\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labuser\Documents\Selenium Session\automation_workspace\EmployeeManagementAutomation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Username</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>bhanu</t>
-  </si>
-  <si>
-    <t>bhanu123</t>
   </si>
   <si>
     <t>Invalid credential</t>
@@ -397,7 +394,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -420,22 +417,22 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>454545</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>